<commit_message>
Added Excel Sheet for new CRC and old CRC
</commit_message>
<xml_diff>
--- a/Documentation/Design/ClassRelationshipCards.xlsx
+++ b/Documentation/Design/ClassRelationshipCards.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>Class Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,37 +35,94 @@
     <t>Template CRC</t>
   </si>
   <si>
-    <t>personalInformation</t>
-  </si>
-  <si>
-    <t>accountBalance</t>
-  </si>
-  <si>
-    <t>loginPassPair</t>
-  </si>
-  <si>
-    <t>Username and Password</t>
-  </si>
-  <si>
-    <t>RedBoxLogin (Interface)</t>
-  </si>
-  <si>
-    <t>Stored Personal Information</t>
-  </si>
-  <si>
-    <t>Stored Account Balance</t>
-  </si>
-  <si>
-    <t>RedBoxUser (Implements RedBoxLogin)</t>
-  </si>
-  <si>
-    <t>adminRights</t>
-  </si>
-  <si>
-    <t>Admin or User</t>
-  </si>
-  <si>
-    <t>RedBoxAdmin</t>
+    <t>Rentable (Interface)</t>
+  </si>
+  <si>
+    <t>Movie (Implements Rentable)</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>VideoGame (Implements Rentable)</t>
+  </si>
+  <si>
+    <t>PersonalInformation</t>
+  </si>
+  <si>
+    <t>User (Implements Login)</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Login (Interface)</t>
+  </si>
+  <si>
+    <t>LoginGUI</t>
+  </si>
+  <si>
+    <t>contain login credentials</t>
+  </si>
+  <si>
+    <t>determine admin access</t>
+  </si>
+  <si>
+    <t>Gathers login credentials</t>
+  </si>
+  <si>
+    <t>Admin (Implements Login)</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>contains rental information</t>
+  </si>
+  <si>
+    <t>contains user information</t>
+  </si>
+  <si>
+    <t>stores personal information</t>
+  </si>
+  <si>
+    <t>RentalInformation</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>store rental information</t>
+  </si>
+  <si>
+    <t>RentableGUI</t>
+  </si>
+  <si>
+    <t>Gathers renting data</t>
+  </si>
+  <si>
+    <t>AccountGUI</t>
+  </si>
+  <si>
+    <t>Shows account information</t>
+  </si>
+  <si>
+    <t>Shows inventory data</t>
+  </si>
+  <si>
+    <t>Gathers account changes</t>
+  </si>
+  <si>
+    <t>UserGUI</t>
+  </si>
+  <si>
+    <t>Shows user options</t>
+  </si>
+  <si>
+    <t>AdminGUI</t>
+  </si>
+  <si>
+    <t>Shows admin options</t>
   </si>
 </sst>
 </file>
@@ -125,16 +179,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,104 +470,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C14"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="8" max="8" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="C10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="H14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="C17" s="4"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="15">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>